<commit_message>
protect spacebar file name
</commit_message>
<xml_diff>
--- a/iLease/test1.xlsx
+++ b/iLease/test1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/autoTest/getTestScript/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/autoTest/iLease/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Confic" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>A0001</t>
   </si>
@@ -75,9 +75,6 @@
     <t>กดที่ ปุ่ม</t>
   </si>
   <si>
-    <t>Para</t>
-  </si>
-  <si>
     <t>ลบค่าใน Input</t>
   </si>
   <si>
@@ -96,24 +93,15 @@
     <t>กดที่พิกัด</t>
   </si>
   <si>
-    <t>x , y</t>
-  </si>
-  <si>
     <t>กดลากนิ้ว</t>
   </si>
   <si>
-    <t>x1, y1, x2, y2</t>
-  </si>
-  <si>
     <t>DELAY</t>
   </si>
   <si>
     <t>หยุดรอ</t>
   </si>
   <si>
-    <t>seconds</t>
-  </si>
-  <si>
     <t>Hub_Cus</t>
   </si>
   <si>
@@ -138,71 +126,77 @@
     <t>x</t>
   </si>
   <si>
+    <t>todoType_14</t>
+  </si>
+  <si>
+    <t>todoItem_0</t>
+  </si>
+  <si>
+    <t>todoItem_1</t>
+  </si>
+  <si>
+    <t>EXPECT</t>
+  </si>
+  <si>
+    <t>ตรวจสอบค่า</t>
+  </si>
+  <si>
+    <t>ID, expect value</t>
+  </si>
+  <si>
+    <t>ID , input text</t>
+  </si>
+  <si>
+    <t>RIGHT</t>
+  </si>
+  <si>
+    <t>WAIT</t>
+  </si>
+  <si>
+    <t>รอโหลด Object</t>
+  </si>
+  <si>
+    <t>187=Switch App , 0=DOWN, 4=Back, 66=Enter</t>
+  </si>
+  <si>
+    <t>KEYCODE</t>
+  </si>
+  <si>
+    <t>Sheet Name</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>IDC_Name_TH</t>
+  </si>
+  <si>
+    <t>บางอ้อ</t>
+  </si>
+  <si>
+    <t>ID, ( overwrite)</t>
+  </si>
+  <si>
+    <t>seconds, ( overwrite)</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>พิกัด  "x , y"</t>
+  </si>
+  <si>
+    <t>พิกัด "x1, y1, x2, y2"</t>
+  </si>
+  <si>
     <t>myyaree@gmail.com</t>
-  </si>
-  <si>
-    <t>todoType_14</t>
-  </si>
-  <si>
-    <t>todoItem_0</t>
-  </si>
-  <si>
-    <t>todoItem_1</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>ID , # กรณีกด Dynamic list</t>
-  </si>
-  <si>
-    <t>EXPECT</t>
-  </si>
-  <si>
-    <t>ตรวจสอบค่า</t>
-  </si>
-  <si>
-    <t>ID, expect value</t>
-  </si>
-  <si>
-    <t>ID , input text</t>
-  </si>
-  <si>
-    <t>IRR</t>
-  </si>
-  <si>
-    <t>RIGHT</t>
-  </si>
-  <si>
-    <t>DOWN</t>
-  </si>
-  <si>
-    <t>WAIT</t>
-  </si>
-  <si>
-    <t>submit_button</t>
-  </si>
-  <si>
-    <t>รอโหลด Object</t>
-  </si>
-  <si>
-    <t>187=Switch App , 0=DOWN, 4=Back, 66=Enter</t>
-  </si>
-  <si>
-    <t>KEYCODE</t>
-  </si>
-  <si>
-    <t>Sheet Name</t>
-  </si>
-  <si>
-    <t>Sheet1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -217,8 +211,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,6 +238,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFECEBED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -250,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -259,12 +266,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFECEBED"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -536,158 +558,511 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="4.83203125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="9" max="9" width="53.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="C1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="I1" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="8">
+        <v>300</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="13">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="8">
+        <v>120</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="13">
+        <v>2</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="13">
+        <v>3</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
-        <v>300</v>
-      </c>
-      <c r="C3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="I5" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="13">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="G6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="13">
+        <v>5</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4">
-        <v>120</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="I7" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="13">
         <v>6</v>
       </c>
-      <c r="I4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G5" t="s">
+      <c r="G8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="13">
+        <v>7</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="13">
+        <v>8</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="13">
         <v>9</v>
       </c>
-      <c r="I5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G6" t="s">
+      <c r="G11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="13">
         <v>10</v>
       </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" t="s">
-        <v>51</v>
-      </c>
-      <c r="K7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" t="s">
-        <v>44</v>
-      </c>
+      <c r="G12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -696,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -711,9 +1086,9 @@
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="2" t="s">
@@ -735,89 +1110,77 @@
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="6"/>
       <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="I2" s="5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
       <c r="H3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4">
-        <v>11.2324</v>
+        <v>34</v>
+      </c>
+      <c r="I4">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>